<commit_message>
git commit -m "script novo: verificar se código de cadastro está com a imagem ok."
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joab.alves\Desktop\automacoes_atacadao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2267EF71-580C-40CD-8BF1-383A00B6FE30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D79ACFD9-01D1-41DC-946F-B37A38348A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{6496AE3B-6423-4F19-A2F2-4933CF75A895}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6496AE3B-6423-4F19-A2F2-4933CF75A895}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="5" r:id="rId1"/>
@@ -36,12 +36,396 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
   <si>
     <t>mpn</t>
   </si>
   <si>
-    <t>C-3377</t>
+    <t>3341283AP</t>
+  </si>
+  <si>
+    <t>A8952AP</t>
+  </si>
+  <si>
+    <t>A8957AP</t>
+  </si>
+  <si>
+    <t>3344243AP</t>
+  </si>
+  <si>
+    <t>228561X</t>
+  </si>
+  <si>
+    <t>R11154</t>
+  </si>
+  <si>
+    <t>R11123</t>
+  </si>
+  <si>
+    <t>01116475-4</t>
+  </si>
+  <si>
+    <t>01116477-4</t>
+  </si>
+  <si>
+    <t>01405981-5</t>
+  </si>
+  <si>
+    <t>V1003</t>
+  </si>
+  <si>
+    <t>01476216-5</t>
+  </si>
+  <si>
+    <t>01846636-4</t>
+  </si>
+  <si>
+    <t>01776318-4</t>
+  </si>
+  <si>
+    <t>01116461-5</t>
+  </si>
+  <si>
+    <t>01919170-5</t>
+  </si>
+  <si>
+    <t>R04011</t>
+  </si>
+  <si>
+    <t>R04710</t>
+  </si>
+  <si>
+    <t>R04708</t>
+  </si>
+  <si>
+    <t>R04012</t>
+  </si>
+  <si>
+    <t>R04075</t>
+  </si>
+  <si>
+    <t>02008465-4</t>
+  </si>
+  <si>
+    <t>01369558-4</t>
+  </si>
+  <si>
+    <t>01369559-4</t>
+  </si>
+  <si>
+    <t>01373174-5</t>
+  </si>
+  <si>
+    <t>01476234-5</t>
+  </si>
+  <si>
+    <t>00378633-5</t>
+  </si>
+  <si>
+    <t>01476272-5</t>
+  </si>
+  <si>
+    <t>V908</t>
+  </si>
+  <si>
+    <t>V975</t>
+  </si>
+  <si>
+    <t>181723BN</t>
+  </si>
+  <si>
+    <t>181711BN</t>
+  </si>
+  <si>
+    <t>161722PK</t>
+  </si>
+  <si>
+    <t>161710PK</t>
+  </si>
+  <si>
+    <t>JL59926</t>
+  </si>
+  <si>
+    <t>961008530034E</t>
+  </si>
+  <si>
+    <t>59626CB</t>
+  </si>
+  <si>
+    <t>71125B</t>
+  </si>
+  <si>
+    <t>77026B</t>
+  </si>
+  <si>
+    <t>70426CB</t>
+  </si>
+  <si>
+    <t>71126CB14</t>
+  </si>
+  <si>
+    <t>48425NA</t>
+  </si>
+  <si>
+    <t>71426B</t>
+  </si>
+  <si>
+    <t>48953F</t>
+  </si>
+  <si>
+    <t>48853EF</t>
+  </si>
+  <si>
+    <t>71277NA</t>
+  </si>
+  <si>
+    <t>71265NA</t>
+  </si>
+  <si>
+    <t>13360NA</t>
+  </si>
+  <si>
+    <t>71165NA</t>
+  </si>
+  <si>
+    <t>48853AN</t>
+  </si>
+  <si>
+    <t>48953AN</t>
+  </si>
+  <si>
+    <t>11930AN</t>
+  </si>
+  <si>
+    <t>JL016123</t>
+  </si>
+  <si>
+    <t>48627PV</t>
+  </si>
+  <si>
+    <t>71627AN</t>
+  </si>
+  <si>
+    <t>71987NT</t>
+  </si>
+  <si>
+    <t>71127PP</t>
+  </si>
+  <si>
+    <t>73027NA</t>
+  </si>
+  <si>
+    <t>70316NAEMBPCH</t>
+  </si>
+  <si>
+    <t>59116PV</t>
+  </si>
+  <si>
+    <t>71116PVEMBPCH</t>
+  </si>
+  <si>
+    <t>71716NA</t>
+  </si>
+  <si>
+    <t>71916AN</t>
+  </si>
+  <si>
+    <t>71917AN</t>
+  </si>
+  <si>
+    <t>60317BO</t>
+  </si>
+  <si>
+    <t>161944NA</t>
+  </si>
+  <si>
+    <t>48419NAEMBPCH</t>
+  </si>
+  <si>
+    <t>48838NA</t>
+  </si>
+  <si>
+    <t>71232NA</t>
+  </si>
+  <si>
+    <t>48838AN</t>
+  </si>
+  <si>
+    <t>60280ML</t>
+  </si>
+  <si>
+    <t>60601SC</t>
+  </si>
+  <si>
+    <t>151558PK</t>
+  </si>
+  <si>
+    <t>171522PK</t>
+  </si>
+  <si>
+    <t>161506PK</t>
+  </si>
+  <si>
+    <t>171530PK</t>
+  </si>
+  <si>
+    <t>171529PK</t>
+  </si>
+  <si>
+    <t>171506MP</t>
+  </si>
+  <si>
+    <t>19151004PK</t>
+  </si>
+  <si>
+    <t>161520PK</t>
+  </si>
+  <si>
+    <t>171508PK</t>
+  </si>
+  <si>
+    <t>19151007PK</t>
+  </si>
+  <si>
+    <t>48802FPSD4</t>
+  </si>
+  <si>
+    <t>181509PK3</t>
+  </si>
+  <si>
+    <t>181507PK3</t>
+  </si>
+  <si>
+    <t>181523PK3</t>
+  </si>
+  <si>
+    <t>161522PK</t>
+  </si>
+  <si>
+    <t>151509PK30</t>
+  </si>
+  <si>
+    <t>15154001ML3</t>
+  </si>
+  <si>
+    <t>161524ML</t>
+  </si>
+  <si>
+    <t>161545ML</t>
+  </si>
+  <si>
+    <t>161531ML</t>
+  </si>
+  <si>
+    <t>161544ML</t>
+  </si>
+  <si>
+    <t>19151206ML</t>
+  </si>
+  <si>
+    <t>161540ML</t>
+  </si>
+  <si>
+    <t>19151020ML</t>
+  </si>
+  <si>
+    <t>15154001ML1</t>
+  </si>
+  <si>
+    <t>151509ML1</t>
+  </si>
+  <si>
+    <t>181530ML3</t>
+  </si>
+  <si>
+    <t>181529ML</t>
+  </si>
+  <si>
+    <t>JL48522AL</t>
+  </si>
+  <si>
+    <t>71121NS</t>
+  </si>
+  <si>
+    <t>73837NA</t>
+  </si>
+  <si>
+    <t>59324CV</t>
+  </si>
+  <si>
+    <t>60422AN</t>
+  </si>
+  <si>
+    <t>71122FS</t>
+  </si>
+  <si>
+    <t>43021NS</t>
+  </si>
+  <si>
+    <t>48321NS</t>
+  </si>
+  <si>
+    <t>48427CV</t>
+  </si>
+  <si>
+    <t>70621S</t>
+  </si>
+  <si>
+    <t>59922FF</t>
+  </si>
+  <si>
+    <t>48020CV</t>
+  </si>
+  <si>
+    <t>941088530334E</t>
+  </si>
+  <si>
+    <t>73932OR</t>
+  </si>
+  <si>
+    <t>60678SC</t>
+  </si>
+  <si>
+    <t>48619NA</t>
+  </si>
+  <si>
+    <t>51525B</t>
+  </si>
+  <si>
+    <t>8PK1410HD</t>
+  </si>
+  <si>
+    <t>13A1350HD</t>
+  </si>
+  <si>
+    <t>8PK1600HD</t>
+  </si>
+  <si>
+    <t>13A0965HD</t>
+  </si>
+  <si>
+    <t>8PK1550HD</t>
+  </si>
+  <si>
+    <t>8PK1400HD</t>
+  </si>
+  <si>
+    <t>10A1200HD</t>
+  </si>
+  <si>
+    <t>8PK1385HD</t>
+  </si>
+  <si>
+    <t>8PK2085HD</t>
+  </si>
+  <si>
+    <t>8PK2020HD</t>
+  </si>
+  <si>
+    <t>8PK1615HD</t>
+  </si>
+  <si>
+    <t>9PK2338HD</t>
   </si>
 </sst>
 </file>
@@ -77,8 +461,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,22 +800,1098 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CA40448-48DE-472D-8B16-D6F43DE709CF}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A217"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="1" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3361824</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>26022</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>6350066</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>14330104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>14330290</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14330100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>14330291</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>14330053</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>14330287</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>14330435</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>14330329</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>14330301</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>14330432</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>1932359</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>1932624</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>1932116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>1932235</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>1932146</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>1932726</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>10330326</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>10330762</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>10330445</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>11330009</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>10330622</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>10330456</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>11330037</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>4304062</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>10330680</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>4301528</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>10330761</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>10330357</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>10330662</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>10330003</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>10330532</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>10350015</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>10350596</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>3344769</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>10330683</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>4308550</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>4304543</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>91210</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>10330372</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>10330714</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>91304120</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>10330414</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>10330599</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>10330205</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>3364011</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>81600060</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>81600200</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>81600210</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>81600240</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>156352</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>903180</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>600862</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>280623</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>768820</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <v>8891</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="1">
+        <v>1733083</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <v>593380</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <v>698630</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
+        <v>451611</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <v>96305</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
+        <v>122581</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="1">
+        <v>740331</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="1">
+        <v>3283569</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="1">
+        <v>763012</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="1">
+        <v>82259</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="1">
+        <v>492905</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="1">
+        <v>99924</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="1">
+        <v>490591</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="1">
+        <v>373240</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="1">
+        <v>402002</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="1">
+        <v>38630</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="1">
+        <v>401410</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="1">
+        <v>152140</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="1">
+        <v>470290</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="1">
+        <v>489870</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="1">
+        <v>8951</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="1">
+        <v>277762</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="1">
+        <v>186140</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="1">
+        <v>475170</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="1">
+        <v>412603</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="1">
+        <v>193711011</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="1">
+        <v>381924</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" s="1">
+        <v>36340</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" s="1">
+        <v>215071</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>